<commit_message>
Corrigido bug no mês anterior
</commit_message>
<xml_diff>
--- a/mapeamento_cc.xlsx
+++ b/mapeamento_cc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Contabil\msc-conferencia2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D0B76D-A4BE-46A2-8C58-9B5A98DC677A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870A5AB9-C3B1-4561-9BA5-F2EF169C028E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,10 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,8 +127,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}" name="tblMapeamentoCC" displayName="tblMapeamentoCC" ref="A1:E1217" totalsRowShown="0">
-  <autoFilter ref="A1:E1217" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}" name="tblMapeamentoCC" displayName="tblMapeamentoCC" ref="A1:E1232" totalsRowShown="0">
+  <autoFilter ref="A1:E1232" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5F1BB400-D3C8-4159-AE93-947471709848}" name="cc_pad" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E3C59A09-EE65-4698-A996-F4FEC4897F1C}" name="cc_msc" dataDxfId="3"/>
@@ -408,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1217"/>
+  <dimension ref="A1:E1232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="B387" sqref="B387:B389"/>
+    <sheetView tabSelected="1" topLeftCell="A1202" workbookViewId="0">
+      <selection activeCell="B1218" sqref="B1218:B1232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24759,6 +24760,306 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1218" s="1">
+        <v>853240101000000</v>
+      </c>
+      <c r="B1218" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1218" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240101</v>
+      </c>
+      <c r="D1218" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1218" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1219" s="1">
+        <v>853240102000000</v>
+      </c>
+      <c r="B1219" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1219" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240102</v>
+      </c>
+      <c r="D1219" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1219" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1220" s="1">
+        <v>853240103000000</v>
+      </c>
+      <c r="B1220" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1220" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240103</v>
+      </c>
+      <c r="D1220" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1220" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1221" s="1">
+        <v>853240201000000</v>
+      </c>
+      <c r="B1221" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1221" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240201</v>
+      </c>
+      <c r="D1221" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1221" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1222" s="1">
+        <v>853240202000000</v>
+      </c>
+      <c r="B1222" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1222" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240202</v>
+      </c>
+      <c r="D1222" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1222" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1223" s="1">
+        <v>853240203000000</v>
+      </c>
+      <c r="B1223" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1223" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240203</v>
+      </c>
+      <c r="D1223" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1223" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1224" s="1">
+        <v>853240204000000</v>
+      </c>
+      <c r="B1224" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1224" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240204</v>
+      </c>
+      <c r="D1224" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1224" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1225" s="1">
+        <v>853240205000000</v>
+      </c>
+      <c r="B1225" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1225" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240205</v>
+      </c>
+      <c r="D1225" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1225" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1226" s="1">
+        <v>853240206000000</v>
+      </c>
+      <c r="B1226" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1226" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240206</v>
+      </c>
+      <c r="D1226" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1226" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1227" s="1">
+        <v>853240300000000</v>
+      </c>
+      <c r="B1227" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1227" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240300</v>
+      </c>
+      <c r="D1227" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1227" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1228" s="1">
+        <v>853240400000000</v>
+      </c>
+      <c r="B1228" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1228" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240400</v>
+      </c>
+      <c r="D1228" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1228" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1229" s="1">
+        <v>853240500000000</v>
+      </c>
+      <c r="B1229" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1229" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240500</v>
+      </c>
+      <c r="D1229" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1229" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1230" s="1">
+        <v>853240600000000</v>
+      </c>
+      <c r="B1230" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1230" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240600</v>
+      </c>
+      <c r="D1230" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1230" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1231" s="1">
+        <v>853240700000000</v>
+      </c>
+      <c r="B1231" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1231" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240700</v>
+      </c>
+      <c r="D1231" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1231" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1232" s="1">
+        <v>853240800000000</v>
+      </c>
+      <c r="B1232" s="2">
+        <v>853240000</v>
+      </c>
+      <c r="C1232" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>853240800</v>
+      </c>
+      <c r="D1232" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>0</v>
+      </c>
+      <c r="E1232" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Padronização de pontos de entrada da aplicação.
</commit_message>
<xml_diff>
--- a/mapeamento_cc.xlsx
+++ b/mapeamento_cc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Contabil\msc-conferencia2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D3ED0E-EFA8-4392-B3E4-5B32F34E28DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68135A8B-D4E8-4333-A72B-E206748C0BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1695" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapCC" sheetId="1" r:id="rId1"/>
@@ -88,10 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,8 +127,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}" name="tblMapeamentoCC" displayName="tblMapeamentoCC" ref="A1:E1805" totalsRowShown="0">
-  <autoFilter ref="A1:E1805" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}" name="tblMapeamentoCC" displayName="tblMapeamentoCC" ref="A1:E1806" totalsRowShown="0">
+  <autoFilter ref="A1:E1806" xr:uid="{E9F3079A-DB93-4A79-9EE8-20034DBF88BC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5F1BB400-D3C8-4159-AE93-947471709848}" name="cc_pad" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E3C59A09-EE65-4698-A996-F4FEC4897F1C}" name="cc_msc" dataDxfId="3"/>
@@ -408,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1805"/>
+  <dimension ref="A1:E1806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1532" workbookViewId="0">
-      <selection activeCell="B1533" sqref="B1533"/>
+    <sheetView tabSelected="1" topLeftCell="A1771" workbookViewId="0">
+      <selection activeCell="B1807" sqref="B1807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36519,6 +36520,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1806" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1806" s="1">
+        <v>521120200000000</v>
+      </c>
+      <c r="B1806" s="2">
+        <v>521120200</v>
+      </c>
+      <c r="C1806" s="2">
+        <f>VALUE(LEFT(tblMapeamentoCC[[#This Row],[cc_pad]],9))</f>
+        <v>521120200</v>
+      </c>
+      <c r="D1806" s="3" t="b">
+        <f>tblMapeamentoCC[[#This Row],[cc_msc]]=tblMapeamentoCC[[#This Row],[padrao]]</f>
+        <v>1</v>
+      </c>
+      <c r="E1806" s="3">
+        <f>COUNTIF(tblMapeamentoCC[cc_pad],tblMapeamentoCC[[#This Row],[cc_pad]])</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>